<commit_message>
FIXED THE NUM PROJS
</commit_message>
<xml_diff>
--- a/assets/projects_directory_main.xlsx
+++ b/assets/projects_directory_main.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SELFWORK_ALW\11_FLORINA_WEBSITE\fdutt3.github.io\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548E23EF-D521-453F-9693-2103E07361E3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3B17956-68DA-4716-949C-062C6C6BE2C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="825" yWindow="-120" windowWidth="37695" windowHeight="16440" xr2:uid="{779BC7F7-762C-45B1-8B7F-93BB33AC0AAF}"/>
   </bookViews>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="478">
   <si>
     <t>proj_id</t>
   </si>
@@ -2074,8 +2074,8 @@
   <dimension ref="A1:N84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2519,6 +2519,9 @@
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="s">
+        <v>440</v>
+      </c>
       <c r="E12" t="s">
         <v>44</v>
       </c>
@@ -2635,6 +2638,9 @@
       <c r="A16">
         <v>15</v>
       </c>
+      <c r="B16" t="s">
+        <v>440</v>
+      </c>
       <c r="E16" t="s">
         <v>57</v>
       </c>
@@ -2660,6 +2666,9 @@
     <row r="17" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>440</v>
       </c>
       <c r="E17" t="s">
         <v>61</v>
@@ -2687,6 +2696,9 @@
       <c r="A18">
         <v>17</v>
       </c>
+      <c r="B18" t="s">
+        <v>440</v>
+      </c>
       <c r="E18" t="s">
         <v>62</v>
       </c>
@@ -2713,6 +2725,9 @@
       <c r="A19">
         <v>18</v>
       </c>
+      <c r="B19" t="s">
+        <v>440</v>
+      </c>
       <c r="E19" t="s">
         <v>65</v>
       </c>
@@ -3714,6 +3729,9 @@
       <c r="A50">
         <v>49</v>
       </c>
+      <c r="B50" t="s">
+        <v>440</v>
+      </c>
       <c r="E50" t="s">
         <v>189</v>
       </c>
@@ -4446,6 +4464,9 @@
       <c r="A74">
         <v>73</v>
       </c>
+      <c r="B74" t="s">
+        <v>440</v>
+      </c>
       <c r="D74" t="s">
         <v>370</v>
       </c>
@@ -4510,6 +4531,9 @@
       <c r="A76">
         <v>75</v>
       </c>
+      <c r="B76" t="s">
+        <v>440</v>
+      </c>
       <c r="D76" t="s">
         <v>370</v>
       </c>
@@ -4626,6 +4650,9 @@
       <c r="A80">
         <v>79</v>
       </c>
+      <c r="B80" t="s">
+        <v>440</v>
+      </c>
       <c r="E80" t="s">
         <v>426</v>
       </c>
@@ -4651,6 +4678,9 @@
     <row r="81" spans="1:14" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>440</v>
       </c>
       <c r="E81" t="s">
         <v>433</v>

</xml_diff>